<commit_message>
Multiples correction sur edition eleve
</commit_message>
<xml_diff>
--- a/resources/FR_TI 2015 - Tableau InscriptionTest.xlsx
+++ b/resources/FR_TI 2015 - Tableau InscriptionTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
   <si>
     <t>N° Club</t>
   </si>
@@ -177,15 +177,6 @@
     <t>Un candidat peut participer au maximum à 2 épreuves Individuelles et 2 épreuves de groupe.</t>
   </si>
   <si>
-    <t>CSMB</t>
-  </si>
-  <si>
-    <t>Gael</t>
-  </si>
-  <si>
-    <t>HENRY</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -198,46 +189,46 @@
     <t>Équipe 1</t>
   </si>
   <si>
-    <t>HUYNH</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>BRUNET</t>
-  </si>
-  <si>
-    <t>Antoine</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
-    <t>Lisa</t>
-  </si>
-  <si>
     <t>Féminin</t>
   </si>
   <si>
-    <t>Marie-Elisabeth</t>
-  </si>
-  <si>
-    <t>MINASYAN</t>
-  </si>
-  <si>
-    <t>Julia</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Test3</t>
+    <t>St Max</t>
+  </si>
+  <si>
+    <t>JJ</t>
+  </si>
+  <si>
+    <t>Test13002001</t>
+  </si>
+  <si>
+    <t>Test13002002</t>
+  </si>
+  <si>
+    <t>Test13002003</t>
+  </si>
+  <si>
+    <t>Test13002004</t>
+  </si>
+  <si>
+    <t>Test13002005</t>
+  </si>
+  <si>
+    <t>Test13002006</t>
+  </si>
+  <si>
+    <t>Test13002007</t>
+  </si>
+  <si>
+    <t>Test13002008</t>
+  </si>
+  <si>
+    <t>Test13002009</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1060,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1292,8 +1283,65 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1364,60 +1412,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="33" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="35" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1599,12 +1593,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2539,24 +2527,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="105"/>
-      <c r="H15" s="105"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
     </row>
     <row r="16" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="105"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="105"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="81"/>
     </row>
     <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
@@ -2569,33 +2557,33 @@
     </row>
     <row r="18" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
-      <c r="C18" s="110" t="s">
+      <c r="C18" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="111"/>
-      <c r="E18" s="116" t="s">
+      <c r="D18" s="87"/>
+      <c r="E18" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="116"/>
-      <c r="G18" s="117"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="93"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
-      <c r="C19" s="114"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="118"/>
-      <c r="F19" s="118"/>
-      <c r="G19" s="119"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="95"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
-      <c r="C20" s="112"/>
-      <c r="D20" s="113"/>
-      <c r="E20" s="120"/>
-      <c r="F20" s="120"/>
-      <c r="G20" s="121"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="97"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -2618,26 +2606,26 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
-      <c r="C23" s="110" t="s">
+      <c r="C23" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="111"/>
-      <c r="E23" s="106" t="s">
+      <c r="D23" s="87"/>
+      <c r="E23" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="106"/>
-      <c r="G23" s="107"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="83"/>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
-      <c r="C24" s="112"/>
-      <c r="D24" s="113"/>
-      <c r="E24" s="108" t="s">
+      <c r="C24" s="88"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="108"/>
-      <c r="G24" s="109"/>
+      <c r="F24" s="84"/>
+      <c r="G24" s="85"/>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -2660,15 +2648,15 @@
     </row>
     <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
-      <c r="C27" s="79" t="s">
+      <c r="C27" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="80"/>
-      <c r="E27" s="81" t="s">
+      <c r="D27" s="99"/>
+      <c r="E27" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="82"/>
-      <c r="G27" s="83"/>
+      <c r="F27" s="101"/>
+      <c r="G27" s="102"/>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -2691,15 +2679,15 @@
     </row>
     <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
-      <c r="C30" s="99" t="s">
+      <c r="C30" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="100"/>
-      <c r="E30" s="101" t="s">
+      <c r="D30" s="119"/>
+      <c r="E30" s="120" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="102"/>
-      <c r="G30" s="103"/>
+      <c r="F30" s="121"/>
+      <c r="G30" s="122"/>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -2722,33 +2710,33 @@
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
-      <c r="C33" s="84" t="s">
+      <c r="C33" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="85"/>
-      <c r="E33" s="90" t="s">
+      <c r="D33" s="104"/>
+      <c r="E33" s="109" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="91"/>
-      <c r="G33" s="92"/>
+      <c r="F33" s="110"/>
+      <c r="G33" s="111"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="93"/>
-      <c r="F34" s="94"/>
-      <c r="G34" s="95"/>
+      <c r="C34" s="105"/>
+      <c r="D34" s="106"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="113"/>
+      <c r="G34" s="114"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
-      <c r="C35" s="88"/>
-      <c r="D35" s="89"/>
-      <c r="E35" s="96"/>
-      <c r="F35" s="97"/>
-      <c r="G35" s="98"/>
+      <c r="C35" s="107"/>
+      <c r="D35" s="108"/>
+      <c r="E35" s="115"/>
+      <c r="F35" s="116"/>
+      <c r="G35" s="117"/>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -2897,18 +2885,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="C33:D35"/>
+    <mergeCell ref="E33:G35"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
     <mergeCell ref="B15:H16"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="E24:G24"/>
     <mergeCell ref="C23:D24"/>
     <mergeCell ref="C18:D20"/>
     <mergeCell ref="E18:G20"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="C33:D35"/>
-    <mergeCell ref="E33:G35"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:G30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2920,8 +2908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="82" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2953,122 +2941,122 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23"/>
-      <c r="B1" s="124" t="s">
+      <c r="B1" s="125" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="125"/>
-      <c r="R1" s="125"/>
-      <c r="S1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="126"/>
+      <c r="M1" s="126"/>
+      <c r="N1" s="126"/>
+      <c r="O1" s="126"/>
+      <c r="P1" s="126"/>
+      <c r="Q1" s="126"/>
+      <c r="R1" s="126"/>
+      <c r="S1" s="127"/>
       <c r="U1" s="55"/>
       <c r="V1" s="55"/>
       <c r="W1" s="55"/>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23"/>
-      <c r="B2" s="127"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128"/>
-      <c r="M2" s="128"/>
-      <c r="N2" s="128"/>
-      <c r="O2" s="128"/>
-      <c r="P2" s="128"/>
-      <c r="Q2" s="128"/>
-      <c r="R2" s="128"/>
-      <c r="S2" s="129"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="129"/>
+      <c r="M2" s="129"/>
+      <c r="N2" s="129"/>
+      <c r="O2" s="129"/>
+      <c r="P2" s="129"/>
+      <c r="Q2" s="129"/>
+      <c r="R2" s="129"/>
+      <c r="S2" s="130"/>
       <c r="U2" s="55"/>
       <c r="V2" s="55"/>
       <c r="W2" s="55"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
-      <c r="B3" s="127"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
-      <c r="N3" s="128"/>
-      <c r="O3" s="128"/>
-      <c r="P3" s="128"/>
-      <c r="Q3" s="128"/>
-      <c r="R3" s="128"/>
-      <c r="S3" s="129"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="129"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="129"/>
+      <c r="N3" s="129"/>
+      <c r="O3" s="129"/>
+      <c r="P3" s="129"/>
+      <c r="Q3" s="129"/>
+      <c r="R3" s="129"/>
+      <c r="S3" s="130"/>
       <c r="U3" s="55"/>
       <c r="V3" s="55"/>
       <c r="W3" s="55"/>
     </row>
     <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="128"/>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
-      <c r="K4" s="128"/>
-      <c r="L4" s="128"/>
-      <c r="M4" s="128"/>
-      <c r="N4" s="128"/>
-      <c r="O4" s="128"/>
-      <c r="P4" s="128"/>
-      <c r="Q4" s="128"/>
-      <c r="R4" s="128"/>
-      <c r="S4" s="129"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="129"/>
+      <c r="N4" s="129"/>
+      <c r="O4" s="129"/>
+      <c r="P4" s="129"/>
+      <c r="Q4" s="129"/>
+      <c r="R4" s="129"/>
+      <c r="S4" s="130"/>
       <c r="U4" s="55"/>
       <c r="V4" s="55"/>
       <c r="W4" s="55"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23"/>
-      <c r="B5" s="130"/>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
-      <c r="H5" s="131"/>
-      <c r="I5" s="131"/>
-      <c r="J5" s="131"/>
-      <c r="K5" s="131"/>
-      <c r="L5" s="131"/>
-      <c r="M5" s="131"/>
-      <c r="N5" s="131"/>
-      <c r="O5" s="131"/>
-      <c r="P5" s="131"/>
-      <c r="Q5" s="131"/>
-      <c r="R5" s="131"/>
-      <c r="S5" s="132"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="132"/>
+      <c r="D5" s="132"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="132"/>
+      <c r="G5" s="132"/>
+      <c r="H5" s="132"/>
+      <c r="I5" s="132"/>
+      <c r="J5" s="132"/>
+      <c r="K5" s="132"/>
+      <c r="L5" s="132"/>
+      <c r="M5" s="132"/>
+      <c r="N5" s="132"/>
+      <c r="O5" s="132"/>
+      <c r="P5" s="132"/>
+      <c r="Q5" s="132"/>
+      <c r="R5" s="132"/>
+      <c r="S5" s="133"/>
       <c r="U5" s="55"/>
       <c r="V5" s="55"/>
       <c r="W5" s="55"/>
@@ -3083,25 +3071,25 @@
         <v>0</v>
       </c>
       <c r="C7" s="29">
-        <v>13001</v>
+        <v>13002</v>
       </c>
       <c r="E7" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="141" t="s">
+      <c r="F7" s="142" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="142"/>
-      <c r="H7" s="142"/>
-      <c r="I7" s="142"/>
-      <c r="J7" s="142"/>
-      <c r="K7" s="142"/>
-      <c r="L7" s="142"/>
-      <c r="M7" s="142"/>
-      <c r="N7" s="142"/>
-      <c r="O7" s="142"/>
-      <c r="P7" s="142"/>
-      <c r="Q7" s="143"/>
+      <c r="G7" s="143"/>
+      <c r="H7" s="143"/>
+      <c r="I7" s="143"/>
+      <c r="J7" s="143"/>
+      <c r="K7" s="143"/>
+      <c r="L7" s="143"/>
+      <c r="M7" s="143"/>
+      <c r="N7" s="143"/>
+      <c r="O7" s="143"/>
+      <c r="P7" s="143"/>
+      <c r="Q7" s="144"/>
       <c r="R7" s="45"/>
       <c r="U7" s="55"/>
       <c r="V7" s="55"/>
@@ -3112,25 +3100,25 @@
         <v>16</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E8" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="144" t="s">
+      <c r="F8" s="145" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="145"/>
-      <c r="H8" s="145"/>
-      <c r="I8" s="145"/>
-      <c r="J8" s="145"/>
-      <c r="K8" s="145"/>
-      <c r="L8" s="145"/>
-      <c r="M8" s="145"/>
-      <c r="N8" s="145"/>
-      <c r="O8" s="145"/>
-      <c r="P8" s="145"/>
-      <c r="Q8" s="146"/>
+      <c r="G8" s="146"/>
+      <c r="H8" s="146"/>
+      <c r="I8" s="146"/>
+      <c r="J8" s="146"/>
+      <c r="K8" s="146"/>
+      <c r="L8" s="146"/>
+      <c r="M8" s="146"/>
+      <c r="N8" s="146"/>
+      <c r="O8" s="146"/>
+      <c r="P8" s="146"/>
+      <c r="Q8" s="147"/>
       <c r="R8" s="46"/>
       <c r="U8" s="55"/>
       <c r="V8" s="55"/>
@@ -3141,25 +3129,25 @@
         <v>17</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E9" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="147" t="s">
+      <c r="F9" s="148" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="148"/>
-      <c r="H9" s="148"/>
-      <c r="I9" s="148"/>
-      <c r="J9" s="148"/>
-      <c r="K9" s="148"/>
-      <c r="L9" s="148"/>
-      <c r="M9" s="148"/>
-      <c r="N9" s="148"/>
-      <c r="O9" s="148"/>
-      <c r="P9" s="148"/>
-      <c r="Q9" s="149"/>
+      <c r="G9" s="149"/>
+      <c r="H9" s="149"/>
+      <c r="I9" s="149"/>
+      <c r="J9" s="149"/>
+      <c r="K9" s="149"/>
+      <c r="L9" s="149"/>
+      <c r="M9" s="149"/>
+      <c r="N9" s="149"/>
+      <c r="O9" s="149"/>
+      <c r="P9" s="149"/>
+      <c r="Q9" s="150"/>
       <c r="R9" s="46"/>
       <c r="U9" s="55"/>
       <c r="V9" s="55"/>
@@ -3170,18 +3158,18 @@
         <v>21</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="F10" s="152"/>
-      <c r="G10" s="152"/>
-      <c r="H10" s="152"/>
-      <c r="I10" s="152"/>
-      <c r="J10" s="152"/>
-      <c r="K10" s="152"/>
-      <c r="L10" s="152"/>
-      <c r="M10" s="152"/>
-      <c r="N10" s="152"/>
-      <c r="O10" s="152"/>
-      <c r="P10" s="152"/>
-      <c r="Q10" s="152"/>
+      <c r="F10" s="153"/>
+      <c r="G10" s="153"/>
+      <c r="H10" s="153"/>
+      <c r="I10" s="153"/>
+      <c r="J10" s="153"/>
+      <c r="K10" s="153"/>
+      <c r="L10" s="153"/>
+      <c r="M10" s="153"/>
+      <c r="N10" s="153"/>
+      <c r="O10" s="153"/>
+      <c r="P10" s="153"/>
+      <c r="Q10" s="153"/>
       <c r="R10" s="46"/>
       <c r="U10" s="55"/>
       <c r="V10" s="55"/>
@@ -3194,20 +3182,20 @@
       <c r="C11" s="28"/>
       <c r="D11" s="5"/>
       <c r="E11" s="77"/>
-      <c r="F11" s="155" t="s">
+      <c r="F11" s="156" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="156"/>
-      <c r="H11" s="156"/>
-      <c r="I11" s="156"/>
-      <c r="J11" s="156"/>
-      <c r="K11" s="156"/>
-      <c r="L11" s="156"/>
-      <c r="M11" s="156"/>
-      <c r="N11" s="156"/>
-      <c r="O11" s="156"/>
-      <c r="P11" s="156"/>
-      <c r="Q11" s="156"/>
+      <c r="G11" s="157"/>
+      <c r="H11" s="157"/>
+      <c r="I11" s="157"/>
+      <c r="J11" s="157"/>
+      <c r="K11" s="157"/>
+      <c r="L11" s="157"/>
+      <c r="M11" s="157"/>
+      <c r="N11" s="157"/>
+      <c r="O11" s="157"/>
+      <c r="P11" s="157"/>
+      <c r="Q11" s="157"/>
       <c r="R11" s="47"/>
       <c r="S11" s="5"/>
       <c r="U11" s="55"/>
@@ -3220,39 +3208,39 @@
       <c r="W12" s="55"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B13" s="136" t="s">
+      <c r="B13" s="137" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="137"/>
-      <c r="D13" s="137"/>
-      <c r="E13" s="137"/>
-      <c r="F13" s="137"/>
-      <c r="G13" s="137"/>
-      <c r="H13" s="137"/>
-      <c r="I13" s="137"/>
-      <c r="J13" s="138"/>
-      <c r="K13" s="133" t="s">
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="138"/>
+      <c r="F13" s="138"/>
+      <c r="G13" s="138"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="138"/>
+      <c r="J13" s="139"/>
+      <c r="K13" s="134" t="s">
         <v>10</v>
       </c>
-      <c r="L13" s="134"/>
-      <c r="M13" s="135"/>
-      <c r="N13" s="153" t="s">
+      <c r="L13" s="135"/>
+      <c r="M13" s="136"/>
+      <c r="N13" s="154" t="s">
         <v>30</v>
       </c>
-      <c r="O13" s="154"/>
-      <c r="P13" s="133" t="s">
+      <c r="O13" s="155"/>
+      <c r="P13" s="134" t="s">
         <v>31</v>
       </c>
-      <c r="Q13" s="150"/>
-      <c r="R13" s="151" t="s">
+      <c r="Q13" s="151"/>
+      <c r="R13" s="152" t="s">
         <v>32</v>
       </c>
-      <c r="S13" s="134"/>
-      <c r="T13" s="135"/>
-      <c r="U13" s="139" t="s">
+      <c r="S13" s="135"/>
+      <c r="T13" s="136"/>
+      <c r="U13" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="V13" s="122" t="s">
+      <c r="V13" s="123" t="s">
         <v>40</v>
       </c>
       <c r="W13" s="5"/>
@@ -3315,49 +3303,49 @@
       <c r="T14" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="U14" s="140"/>
-      <c r="V14" s="123"/>
+      <c r="U14" s="141"/>
+      <c r="V14" s="124"/>
       <c r="W14" s="5"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B15" s="30">
         <f>IF(ISBLANK($D15),"",$C$7)</f>
-        <v>13001</v>
+        <v>13002</v>
       </c>
       <c r="C15" s="36" t="str">
         <f>IF(ISBLANK($D15),"",$C$8)</f>
-        <v>CSMB</v>
+        <v>St Max</v>
       </c>
       <c r="D15" s="19">
-        <v>1300101</v>
+        <v>13002001</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F15" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="78">
+        <v>36537</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="19" t="s">
         <v>49</v>
-      </c>
-      <c r="G15" s="78">
-        <v>31</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>52</v>
       </c>
       <c r="J15" s="21"/>
       <c r="K15" s="18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L15" s="19"/>
       <c r="M15" s="21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N15" s="22"/>
       <c r="O15" s="51"/>
       <c r="P15" s="22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Q15" s="22"/>
       <c r="R15" s="51"/>
@@ -3370,42 +3358,42 @@
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B16" s="37">
         <f t="shared" ref="B16:B40" si="0">IF(ISBLANK(D16),"",$C$7)</f>
-        <v>13001</v>
+        <v>13002</v>
       </c>
       <c r="C16" s="36" t="str">
         <f t="shared" ref="C16:C40" si="1">IF(ISBLANK($D16),"",$C$8)</f>
-        <v>CSMB</v>
+        <v>St Max</v>
       </c>
       <c r="D16" s="19">
-        <v>1300102</v>
+        <v>13002002</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G16" s="78">
-        <v>18</v>
+        <v>36418</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J16" s="21"/>
       <c r="K16" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L16" s="6"/>
       <c r="M16" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N16" s="16"/>
       <c r="O16" s="52"/>
       <c r="P16" s="16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Q16" s="16"/>
       <c r="R16" s="51"/>
@@ -3418,42 +3406,42 @@
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" s="37">
         <f t="shared" si="0"/>
-        <v>13001</v>
+        <v>13002</v>
       </c>
       <c r="C17" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>CSMB</v>
+        <v>St Max</v>
       </c>
       <c r="D17" s="19">
-        <v>1300103</v>
+        <v>13002003</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G17" s="78">
-        <v>17</v>
+        <v>29508</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J17" s="21"/>
       <c r="K17" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N17" s="16"/>
       <c r="O17" s="52"/>
       <c r="P17" s="16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Q17" s="16"/>
       <c r="R17" s="51"/>
@@ -3466,35 +3454,35 @@
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18" s="37">
         <f t="shared" si="0"/>
-        <v>13001</v>
+        <v>13002</v>
       </c>
       <c r="C18" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>CSMB</v>
+        <v>St Max</v>
       </c>
       <c r="D18" s="19">
-        <v>1300104</v>
+        <v>13002004</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F18" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="19">
-        <v>17</v>
+      <c r="G18" s="78">
+        <v>30543</v>
       </c>
       <c r="H18" s="7" t="str">
         <f t="shared" ref="H18:H30" si="2">IF(OR(G18=8,G18=9),"P",IF(OR(G18=10,G18=11),"B",IF(OR(G18=12,G18=13),"M",IF(OR(G18=14,G18=15),"C",IF(OR(G18=16,G18=17),"J",IF(AND(G18&gt;17,G18&lt;35),"S",IF(AND(G18&gt;34,G18&lt;50),"V","")))))))</f>
-        <v>J</v>
+        <v/>
       </c>
       <c r="I18" s="19" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="J18" s="21"/>
       <c r="K18" s="9"/>
       <c r="L18" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="16"/>
@@ -3503,7 +3491,7 @@
       <c r="Q18" s="16"/>
       <c r="R18" s="51"/>
       <c r="S18" s="51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="T18" s="51"/>
       <c r="U18" s="52"/>
@@ -3513,38 +3501,38 @@
     <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B19" s="37">
         <f t="shared" si="0"/>
-        <v>13001</v>
+        <v>13002</v>
       </c>
       <c r="C19" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>CSMB</v>
+        <v>St Max</v>
       </c>
       <c r="D19" s="19">
-        <v>1300105</v>
+        <v>13002005</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="19">
-        <v>17</v>
+        <v>61</v>
+      </c>
+      <c r="G19" s="78">
+        <v>32131</v>
       </c>
       <c r="H19" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>J</v>
+        <v/>
       </c>
       <c r="I19" s="19" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="J19" s="21"/>
       <c r="K19" s="9"/>
       <c r="L19" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N19" s="16"/>
       <c r="O19" s="52"/>
@@ -3552,7 +3540,7 @@
       <c r="Q19" s="16"/>
       <c r="R19" s="51"/>
       <c r="S19" s="51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="T19" s="51"/>
       <c r="U19" s="52"/>
@@ -3562,37 +3550,37 @@
     <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B20" s="37">
         <f t="shared" si="0"/>
-        <v>13001</v>
+        <v>13002</v>
       </c>
       <c r="C20" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>CSMB</v>
+        <v>St Max</v>
       </c>
       <c r="D20" s="19">
-        <v>1300106</v>
+        <v>13002006</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="19">
-        <v>15</v>
+        <v>62</v>
+      </c>
+      <c r="G20" s="78">
+        <v>37397</v>
       </c>
       <c r="H20" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>C</v>
+        <v/>
       </c>
       <c r="I20" s="19" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="J20" s="21"/>
       <c r="K20" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M20" s="10"/>
       <c r="N20" s="16"/>
@@ -3601,7 +3589,7 @@
       <c r="Q20" s="16"/>
       <c r="R20" s="51"/>
       <c r="S20" s="51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="T20" s="51"/>
       <c r="U20" s="52"/>
@@ -3611,29 +3599,29 @@
     <row r="21" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B21" s="37">
         <f t="shared" si="0"/>
-        <v>13001</v>
+        <v>13002</v>
       </c>
       <c r="C21" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>CSMB</v>
+        <v>St Max</v>
       </c>
       <c r="D21" s="19">
-        <v>1300107</v>
+        <v>13002007</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="G21" s="169">
-        <v>36683</v>
+        <v>63</v>
+      </c>
+      <c r="G21" s="78">
+        <v>27619</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J21" s="21">
         <v>28</v>
@@ -3645,11 +3633,11 @@
       <c r="O21" s="52"/>
       <c r="P21" s="16"/>
       <c r="Q21" s="16"/>
-      <c r="R21" s="170"/>
+      <c r="R21" s="79"/>
       <c r="S21" s="6"/>
       <c r="T21" s="10"/>
       <c r="U21" s="52" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="V21" s="16"/>
       <c r="W21" s="5"/>
@@ -3657,29 +3645,29 @@
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B22" s="37">
         <f t="shared" si="0"/>
-        <v>13001</v>
+        <v>13002</v>
       </c>
       <c r="C22" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>CSMB</v>
+        <v>St Max</v>
       </c>
       <c r="D22" s="19">
-        <v>1300108</v>
+        <v>13002008</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G22" s="169">
-        <v>36683</v>
+        <v>64</v>
+      </c>
+      <c r="G22" s="78">
+        <v>38700</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J22" s="21">
         <v>32</v>
@@ -3691,11 +3679,11 @@
       <c r="O22" s="52"/>
       <c r="P22" s="16"/>
       <c r="Q22" s="16"/>
-      <c r="R22" s="170"/>
+      <c r="R22" s="79"/>
       <c r="S22" s="6"/>
       <c r="T22" s="10"/>
       <c r="U22" s="52" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="V22" s="16"/>
       <c r="W22" s="5"/>
@@ -3703,29 +3691,29 @@
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B23" s="37">
         <f t="shared" si="0"/>
-        <v>13001</v>
+        <v>13002</v>
       </c>
       <c r="C23" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>CSMB</v>
+        <v>St Max</v>
       </c>
       <c r="D23" s="19">
-        <v>1300109</v>
+        <v>13002009</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="169">
-        <v>36683</v>
+        <v>65</v>
+      </c>
+      <c r="G23" s="78">
+        <v>39341</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J23" s="21">
         <v>60</v>
@@ -3737,11 +3725,11 @@
       <c r="O23" s="52"/>
       <c r="P23" s="16"/>
       <c r="Q23" s="16"/>
-      <c r="R23" s="170"/>
+      <c r="R23" s="79"/>
       <c r="S23" s="6"/>
       <c r="T23" s="10"/>
       <c r="U23" s="52" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="V23" s="16"/>
       <c r="W23" s="5"/>
@@ -5311,45 +5299,45 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56"/>
-      <c r="B1" s="157" t="s">
+      <c r="B1" s="158" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="160"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="56"/>
-      <c r="B2" s="160"/>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
-      <c r="E2" s="161"/>
-      <c r="F2" s="162"/>
+      <c r="B2" s="161"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="163"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="56"/>
-      <c r="B3" s="160"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="162"/>
+      <c r="B3" s="161"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="163"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="56"/>
-      <c r="B4" s="160"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="162"/>
+      <c r="B4" s="161"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="162"/>
+      <c r="F4" s="163"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="56"/>
-      <c r="B5" s="163"/>
-      <c r="C5" s="164"/>
-      <c r="D5" s="164"/>
-      <c r="E5" s="164"/>
-      <c r="F5" s="165"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="165"/>
+      <c r="F5" s="166"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -5394,12 +5382,12 @@
     </row>
     <row r="12" spans="1:6" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="166" t="s">
+      <c r="B13" s="167" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="166"/>
-      <c r="D13" s="166"/>
-      <c r="E13" s="167" t="s">
+      <c r="C13" s="167"/>
+      <c r="D13" s="167"/>
+      <c r="E13" s="168" t="s">
         <v>44</v>
       </c>
       <c r="F13" s="66"/>
@@ -5414,7 +5402,7 @@
       <c r="D14" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="168"/>
+      <c r="E14" s="169"/>
       <c r="F14" s="66"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>